<commit_message>
final files for 6/7
</commit_message>
<xml_diff>
--- a/Analysis packages.xlsx
+++ b/Analysis packages.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristinporter/Library/CloudStorage/OneDrive-K.E.PorterConsultingLLC/Git/Data-WorkRTI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://keporterconsultingllc-my.sharepoint.com/personal/kristinporter_keporterconsultingllc_onmicrosoft_com/Documents/Git/Data-WorkRTI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7125C70B-D8DF-044B-8C81-099EBD3C38BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{7125C70B-D8DF-044B-8C81-099EBD3C38BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F53418E-3BCA-2949-848E-64574128390C}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{375C8780-387F-0C40-B557-D55489D02869}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>ANOVA (Analysis of variance)</t>
   </si>
@@ -379,6 +379,18 @@
   </si>
   <si>
     <t>Package/function/resource</t>
+  </si>
+  <si>
+    <t>Predictive modeling</t>
+  </si>
+  <si>
+    <t>Tidymodels (part of Tidyverse)</t>
+  </si>
+  <si>
+    <t>caret</t>
+  </si>
+  <si>
+    <t>lots of packages for individual maching learning algorithms (e.g. randomForest)</t>
   </si>
 </sst>
 </file>
@@ -458,21 +470,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -808,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC8AAF5-1E7C-2140-8217-BECF019B032B}">
-  <dimension ref="A1:B47"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -822,10 +833,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -862,7 +873,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -870,31 +881,31 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
       <c r="B7" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
       <c r="B8" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="6"/>
       <c r="B9" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
       <c r="B10" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -902,37 +913,37 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
@@ -954,7 +965,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -962,7 +973,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
         <v>24</v>
       </c>
@@ -976,7 +987,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -984,19 +995,19 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
+      <c r="A24" s="7"/>
       <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1004,162 +1015,183 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
+      <c r="A27" s="6"/>
       <c r="B27" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
+      <c r="A28" s="6"/>
       <c r="B28" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="7"/>
-      <c r="B30" s="2" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="7"/>
-      <c r="B31" s="2" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="6"/>
+      <c r="B34" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="7"/>
-      <c r="B32" s="2" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="2" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="4"/>
-      <c r="B35" s="2" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="5"/>
+      <c r="B38" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="4"/>
-      <c r="B36" s="2" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="5"/>
+      <c r="B39" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="4"/>
-      <c r="B40" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="5"/>
+      <c r="B43" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="9" t="s">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="B43" s="2" t="s">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="4" t="s">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="4"/>
-      <c r="B45" s="2" t="s">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="5"/>
+      <c r="B48" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="1" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="1" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A34:A36"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A44:A45"/>
+  <mergeCells count="10">
+    <mergeCell ref="A37:A39"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A47:A48"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A26:A28"/>
-    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A32:A36"/>
     <mergeCell ref="A11:A17"/>
     <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A29:A31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://www.rdocumentation.org/packages/stats/versions/3.6.2/topics/anova" xr:uid="{337CF910-5E7D-DA47-8417-586D5940E481}"/>
@@ -1184,26 +1216,29 @@
     <hyperlink ref="B24" r:id="rId20" display="https://cran.r-project.org/web/packages/ggraph/vignettes/tidygraph.html" xr:uid="{AF80760E-819E-8D40-80DD-45050DC3C50D}"/>
     <hyperlink ref="B25" r:id="rId21" display="https://cran.r-project.org/web/packages/network/vignettes/networkVignette.pdf" xr:uid="{A2ED8212-22E6-3445-8BB1-9791A663B416}"/>
     <hyperlink ref="B26" r:id="rId22" display="https://cran.r-project.org/web/packages/pwr/vignettes/pwr-vignette.html" xr:uid="{2E3730B8-3E68-7448-97D6-24E613754D3F}"/>
-    <hyperlink ref="B29" r:id="rId23" display="https://cran.r-project.org/web/packages/MatchIt/vignettes/MatchIt.html" xr:uid="{25C0AD32-C985-8C43-BCAD-6C54692D77AA}"/>
-    <hyperlink ref="B30" r:id="rId24" display="https://scholarworks.umass.edu/cgi/viewcontent.cgi?article=1340&amp;context=pare" xr:uid="{0C67FF71-CF6E-054A-9777-5724C997D893}"/>
-    <hyperlink ref="B31" r:id="rId25" display="https://scholarworks.umass.edu/cgi/viewcontent.cgi?article=1286&amp;context=pare" xr:uid="{B228D1B2-0F7B-514C-A019-17F95200531E}"/>
-    <hyperlink ref="B32" r:id="rId26" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8246231/" xr:uid="{93028F6D-506B-564A-8488-686CA1DE82F9}"/>
-    <hyperlink ref="B33" r:id="rId27" display="https://www.r-bloggers.com/2022/04/propensity-score-matching/" xr:uid="{C9A2698D-9EE4-DE4A-97BC-6E9ED0256F79}"/>
-    <hyperlink ref="B34" r:id="rId28" display="https://cran.r-project.org/web/packages/rdd/index.html" xr:uid="{8B7842E0-F588-7C48-87BD-F1707242B062}"/>
-    <hyperlink ref="B35" r:id="rId29" display="https://cran.r-project.org/web/packages/rdrobust/index.html" xr:uid="{F5F2289B-9B3E-1A4F-90E8-6BA5ED742973}"/>
-    <hyperlink ref="B36" r:id="rId30" display="https://cran.r-project.org/web/packages/rdd/index.html" xr:uid="{271A2F12-0CDE-3D4B-BD71-98977557DAAA}"/>
-    <hyperlink ref="B37" r:id="rId31" display="https://cran.r-project.org/web/packages/leaps/index.html" xr:uid="{E7DBB1A0-E0AA-7F42-AA85-B4374ACDD5A2}"/>
-    <hyperlink ref="B38" r:id="rId32" display="https://cran.r-project.org/web/packages/relaimpo/index.html" xr:uid="{AF27C9E2-AD4D-F04B-999C-9FABE451D946}"/>
-    <hyperlink ref="B39" r:id="rId33" display="https://cran.r-project.org/web/packages/MASS/index.html" xr:uid="{D4DC8F92-D867-5D48-81F7-DC45B7C5FB4D}"/>
-    <hyperlink ref="B40" r:id="rId34" display="https://cran.r-project.org/web/packages/estimatr/index.html" xr:uid="{78D797F9-5E11-2F4E-B712-73597297F2A6}"/>
-    <hyperlink ref="B42" r:id="rId35" display="https://socialsciences.mcmaster.ca/jfox/Misc/sem/SEM-paper.pdf" xr:uid="{FD1172DF-AC6B-4144-A116-DA0CF5649B10}"/>
-    <hyperlink ref="B43" r:id="rId36" display="https://cran.r-project.org/web/packages/seminr/vignettes/SEMinR.html" xr:uid="{CD03D818-96B9-DB42-9050-FA2C56BD1726}"/>
-    <hyperlink ref="B44" r:id="rId37" display="https://cran.r-project.org/web/packages/survival/vignettes/survival.pdf" xr:uid="{2A4C06CB-91DE-8D40-9596-BC2F41F1182A}"/>
-    <hyperlink ref="B45" r:id="rId38" display="https://mdrc365.sharepoint.com/:v:/r/sites/ResearchTechnologyUnit/Shared Documents/Watch Videos/DPUG/2018_10_25 DPUG 01 Road to Survival Analysis.mp4?csf=1&amp;web=1&amp;e=q5WKoS" xr:uid="{CAA9680F-7D8B-844F-8F52-BABA8B05DD59}"/>
-    <hyperlink ref="B46" r:id="rId39" display="https://www.rdocumentation.org/packages/stats/versions/3.6.2/topics/t.test" xr:uid="{80371493-744B-C344-84B0-4578A854550E}"/>
-    <hyperlink ref="B47" r:id="rId40" display="https://www.rdocumentation.org/packages/stats/versions/3.6.2/topics/ts" xr:uid="{AF957C13-6F23-5544-84EC-E6B214A2E4BF}"/>
+    <hyperlink ref="B32" r:id="rId23" display="https://cran.r-project.org/web/packages/MatchIt/vignettes/MatchIt.html" xr:uid="{25C0AD32-C985-8C43-BCAD-6C54692D77AA}"/>
+    <hyperlink ref="B33" r:id="rId24" display="https://scholarworks.umass.edu/cgi/viewcontent.cgi?article=1340&amp;context=pare" xr:uid="{0C67FF71-CF6E-054A-9777-5724C997D893}"/>
+    <hyperlink ref="B34" r:id="rId25" display="https://scholarworks.umass.edu/cgi/viewcontent.cgi?article=1286&amp;context=pare" xr:uid="{B228D1B2-0F7B-514C-A019-17F95200531E}"/>
+    <hyperlink ref="B35" r:id="rId26" display="https://www.ncbi.nlm.nih.gov/pmc/articles/PMC8246231/" xr:uid="{93028F6D-506B-564A-8488-686CA1DE82F9}"/>
+    <hyperlink ref="B36" r:id="rId27" display="https://www.r-bloggers.com/2022/04/propensity-score-matching/" xr:uid="{C9A2698D-9EE4-DE4A-97BC-6E9ED0256F79}"/>
+    <hyperlink ref="B37" r:id="rId28" display="https://cran.r-project.org/web/packages/rdd/index.html" xr:uid="{8B7842E0-F588-7C48-87BD-F1707242B062}"/>
+    <hyperlink ref="B38" r:id="rId29" display="https://cran.r-project.org/web/packages/rdrobust/index.html" xr:uid="{F5F2289B-9B3E-1A4F-90E8-6BA5ED742973}"/>
+    <hyperlink ref="B39" r:id="rId30" display="https://cran.r-project.org/web/packages/rdd/index.html" xr:uid="{271A2F12-0CDE-3D4B-BD71-98977557DAAA}"/>
+    <hyperlink ref="B40" r:id="rId31" display="https://cran.r-project.org/web/packages/leaps/index.html" xr:uid="{E7DBB1A0-E0AA-7F42-AA85-B4374ACDD5A2}"/>
+    <hyperlink ref="B41" r:id="rId32" display="https://cran.r-project.org/web/packages/relaimpo/index.html" xr:uid="{AF27C9E2-AD4D-F04B-999C-9FABE451D946}"/>
+    <hyperlink ref="B42" r:id="rId33" display="https://cran.r-project.org/web/packages/MASS/index.html" xr:uid="{D4DC8F92-D867-5D48-81F7-DC45B7C5FB4D}"/>
+    <hyperlink ref="B43" r:id="rId34" display="https://cran.r-project.org/web/packages/estimatr/index.html" xr:uid="{78D797F9-5E11-2F4E-B712-73597297F2A6}"/>
+    <hyperlink ref="B45" r:id="rId35" display="https://socialsciences.mcmaster.ca/jfox/Misc/sem/SEM-paper.pdf" xr:uid="{FD1172DF-AC6B-4144-A116-DA0CF5649B10}"/>
+    <hyperlink ref="B46" r:id="rId36" display="https://cran.r-project.org/web/packages/seminr/vignettes/SEMinR.html" xr:uid="{CD03D818-96B9-DB42-9050-FA2C56BD1726}"/>
+    <hyperlink ref="B47" r:id="rId37" display="https://cran.r-project.org/web/packages/survival/vignettes/survival.pdf" xr:uid="{2A4C06CB-91DE-8D40-9596-BC2F41F1182A}"/>
+    <hyperlink ref="B48" r:id="rId38" display="https://mdrc365.sharepoint.com/:v:/r/sites/ResearchTechnologyUnit/Shared Documents/Watch Videos/DPUG/2018_10_25 DPUG 01 Road to Survival Analysis.mp4?csf=1&amp;web=1&amp;e=q5WKoS" xr:uid="{CAA9680F-7D8B-844F-8F52-BABA8B05DD59}"/>
+    <hyperlink ref="B49" r:id="rId39" display="https://www.rdocumentation.org/packages/stats/versions/3.6.2/topics/t.test" xr:uid="{80371493-744B-C344-84B0-4578A854550E}"/>
+    <hyperlink ref="B50" r:id="rId40" display="https://www.rdocumentation.org/packages/stats/versions/3.6.2/topics/ts" xr:uid="{AF957C13-6F23-5544-84EC-E6B214A2E4BF}"/>
     <hyperlink ref="B27" r:id="rId41" xr:uid="{DE8E4465-384C-7643-B4B8-04EF6A30D9B9}"/>
     <hyperlink ref="B28" r:id="rId42" display="PUMP" xr:uid="{C66B2C0C-4196-4149-B302-FDEB24FF6588}"/>
+    <hyperlink ref="B29" r:id="rId43" xr:uid="{C45AC346-2758-F543-B0A5-D6E663EF1313}"/>
+    <hyperlink ref="B31" r:id="rId44" xr:uid="{28677CCE-F4E4-604A-961B-705640D74611}"/>
+    <hyperlink ref="B30" r:id="rId45" xr:uid="{6D21BF21-0CED-5D4D-B344-9123BCE629D7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>